<commit_message>
Data preparation & Rolling Regression
</commit_message>
<xml_diff>
--- a/Dataset/NASDAQ_INDEX.xlsx
+++ b/Dataset/NASDAQ_INDEX.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d4a6bc32fec4062/UNIMIB_DataScience/99-PROJECTS/FinancialMarketAnalytics2022/Financial_Market_Analytics/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11B4B5A-D082-4B85-897A-31ACE8EC370B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{B11B4B5A-D082-4B85-897A-31ACE8EC370B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D6BAA21-B7B1-42C9-A148-9B77D3F1947B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,10 +416,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B1262"/>
+  <dimension ref="A1:B1261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10516,15 +10516,10 @@
         <v>12125.69</v>
       </c>
     </row>
-    <row r="1262" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1262" s="2">
-        <v>44753</v>
-      </c>
-      <c r="B1262" s="3">
-        <v>11965.27</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B1262">
+    <sortCondition ref="A1:A1262"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>